<commit_message>
updated pre and post test alerts
</commit_message>
<xml_diff>
--- a/thiopurines/Thiopurines_Pre_and_Post_Test_Alerts_and_Flow_Chart.xlsx
+++ b/thiopurines/Thiopurines_Pre_and_Post_Test_Alerts_and_Flow_Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwc/Dropbox/MWC_transfer/CPIC/guidelines/thiopurine_CPIC/2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941C5D36-4231-C341-9079-BAD445C03021}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4843AA9A-FE6D-7B47-A3BE-30BFD114A233}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24700" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-880" yWindow="1980" windowWidth="25240" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pre- and Post-test alerts" sheetId="14" r:id="rId1"/>
@@ -389,14 +389,6 @@
     <t>6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be a NUDT15 normal metabolizer; there is no reason to selectively adjust the dose of this medication based on the NUDT15 result. Because a TPMT genotype does not appear to have been ordered for this patient, it is not known if TPMT results would influence the recommended dose or drug.  Please consult a clinical pharmacist for more information.</t>
   </si>
   <si>
-    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be a possible NUDT15 intermediate metabolizer and is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-70% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g. start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Because a TPMT genotype does not appear to have been ordered for this patient, it is not known if TPMT results would further influence the recommended dose or drug.  Please consult a clinical pharmacist for more information.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be a NUDT15 intermediate metabolizer and is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-70% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended. Because a TPMT genotype does not appear to have been ordered for this patient, it is not known if TPMT results would further influence the recommended dose or drug.  Please consult a clinical pharmacist for more information.
-</t>
-  </si>
-  <si>
     <t>Azathioprine can be affected by a patient’s TPMT and NUDT15 phenotype. Neither a TPMT or NUDT15 genotype appears to have been ordered for this patient. Based on those results, use of an alternative dose or drug may be recommended. Please consult a clinical pharmacist for more information.</t>
   </si>
   <si>
@@ -437,63 +429,25 @@
     <t>Azathioprine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be a TPMT normal metabolizer; there is no reason to selectively adjust the dose of this medication based on the TPMT result. Because a NUDT15 genotype does not appear to have been ordered for this patient, it is not known if NUDT15 results would further influence the recommended dose or drug. Please consult a clinical pharmacist for more information.</t>
   </si>
   <si>
-    <t>6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be a TPMT normal metabolizer and NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-70% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.</t>
-  </si>
-  <si>
     <t>Azathioprine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be a TPMT normal metabolizer and NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of azathioprine. Start with reduced starting doses (30%-80% of normal dose) if normal starting dose is 2-3 mg/kg/day, (e.g. 0.6 – 2.4 mg/kg/day), and adjust doses of azathioprine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment.  Please consult a clinical pharmacist for more information.</t>
   </si>
   <si>
-    <t>6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be a  TPMT normal metabolizer and possible NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-70% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g. start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.</t>
-  </si>
-  <si>
     <t>Azathioprine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be a TPMT normal metabolizer and NUDT15 poor metabolizer. This patient is at high risk for life threatening myelosuppression with normal doses of azathioprine and should receive greatly reduced doses. For non-malignant conditions, consider alternative non-thiopurine immunosuppressant therapy. For malignant conditions, start with drastically reduced normal daily doses (reduce daily dose by 10 fold and dose thrice weekly instead of daily) and adjust doses of azathioprine based on degree of myelosuppression and disease-specific guidelines. Allow 4-6 weeks to reach steady-state after each dose adjustment.    Please consult a clinical pharmacist for more information.</t>
   </si>
   <si>
-    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be TPMT intermediate metabolizer and is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-70% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g. start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended. Because a NUDT15 genotype does not appear to have been ordered for this patient,  it is not known if NUDT15 results would further influence the recommended dose or drug. Please consult a clinical pharmacist for more information.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be TPMT intermediate metabolizer and NUDT15 normal metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-70% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be TPMT intermediate metabolizer and NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-70% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines.  Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Azathioprine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be TPMT intermediate metabolizer and NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of azathioprine. Start with reduced starting doses (30%-80% of normal dose) if normal starting dose is 2-3 mg/kg/day, (e.g. 0.6 – 2.4 mg/kg/day), and adjust doses of azathioprine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. Please consult a clinical pharmacist for more information.
 </t>
   </si>
   <si>
-    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be TPMT intermediate metabolizer and possible NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-70% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Azathioprine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be TPMT intermediate metabolizer and possible NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of azathioprine. Start with reduced starting doses (30%-80% of normal dose) if normal starting dose is 2-3 mg/kg/day, (e.g. 0.6 – 2.4 mg/kg/day), and adjust doses of azathioprine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. Please consult a clinical pharmacist for more information.
 </t>
   </si>
   <si>
-    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be possible TPMT intermediate metabolizer and is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-70% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g. start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended. Because a NUDT15 genotype does not appear to have been ordered for this patient,  it is not known if NUDT15 results would further influence the recommended dose or drug. Please consult a clinical pharmacist for more information.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be possible TPMT intermediate metabolizer and NUDT15 normal metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-70% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Azathioprine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be possible TPMT intermediate metabolizer and NUDT15 normal metabolizer. This patient is at risk for myelosuppression with normal doses of azathioprine. Start with reduced starting doses (30%-80% of normal dose) if normal starting dose is 2-3 mg/kg/day, (e.g. 0.6 – 2.4 mg/kg/day), and adjust doses of azathioprine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. Please consult a clinical pharmacist for more information.
 </t>
   </si>
   <si>
-    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be possible TPMT intermediate metabolizer and NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-70% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines.  Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Azathioprine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be possible TPMT intermediate metabolizer and NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of azathioprine. Start with reduced starting doses (30%-80% of normal dose) if normal starting dose is 2-3 mg/kg/day, (e.g. 0.6 – 2.4 mg/kg/day), and adjust doses of azathioprine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. Please consult a clinical pharmacist for more information.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be possible TPMT intermediate metabolizer and possible NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-70% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.
 </t>
   </si>
   <si>
@@ -745,6 +699,52 @@
       </rPr>
       <t xml:space="preserve"> and adjust doses of thioguanine based on degree of myelosuppression and disease-specific guidelines. Allow 4-6 weeks to reach steady-state after each dose adjustment. In setting of myelosuppression, emphasis should be on reducing thioguanine over other agents.For non-malignant conditions, consider alternative non-thiopurine immunosuppressant therapy. Please consult a clinical pharmacist for more information.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be a NUDT15 intermediate metabolizer and is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-80% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended. Because a TPMT genotype does not appear to have been ordered for this patient, it is not known if TPMT results would further influence the recommended dose or drug.  Please consult a clinical pharmacist for more information.
+</t>
+  </si>
+  <si>
+    <t>6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be a TPMT normal metabolizer and NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-80% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be TPMT intermediate metabolizer and is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-80% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g. start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended. Because a NUDT15 genotype does not appear to have been ordered for this patient,  it is not known if NUDT15 results would further influence the recommended dose or drug. Please consult a clinical pharmacist for more information.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be TPMT intermediate metabolizer and NUDT15 normal metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-80% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be TPMT intermediate metabolizer and NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-80% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines.  Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be TPMT intermediate metabolizer and possible NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-80% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.
+</t>
+  </si>
+  <si>
+    <t>6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be a  TPMT normal metabolizer and possible NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-80% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g. start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be possible TPMT intermediate metabolizer and is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-80% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g. start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended. Because a NUDT15 genotype does not appear to have been ordered for this patient,  it is not known if NUDT15 results would further influence the recommended dose or drug. Please consult a clinical pharmacist for more information.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be possible TPMT intermediate metabolizer and NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-80% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines.  Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be possible TPMT intermediate metabolizer and possible NUDT15 intermediate metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-80% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be possible TPMT intermediate metabolizer and NUDT15 normal metabolizer. This patient is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-80% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g., start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Please consult a clinical pharmacist for more information.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-mercaptopurine can be affected by a patient’s TPMT and NUDT15 phenotype. This patient is predicted to be a possible NUDT15 intermediate metabolizer and is at risk for myelosuppression with normal doses of 6-mercaptopurine. Consider starting 6-mercaptopurine at 30-80% of normal dose if normal starting dose is ≥75 mg/m2/day or ≥ 1.5 mg/kg/day  (e.g. start at 25-60 mg/m2/day or 0.45-1.2 mg/kg/day) and adjust doses of mercaptopurine based on degree of myelosuppression and disease-specific guidelines. Allow 2-4 weeks to reach steady-state after each dose adjustment. If myelosuppression occurs, and depending on other therapy, emphasis should be on reducing mercaptopurine over other agents. If normal starting dose is already &lt;75mg/m2/day or &lt; 1.5mg/kg/day, dose reduction may not be recommended.  Because a TPMT genotype does not appear to have been ordered for this patient, it is not known if TPMT results would further influence the recommended dose or drug.  Please consult a clinical pharmacist for more information.
+</t>
   </si>
 </sst>
 </file>
@@ -1132,6 +1132,30 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1157,30 +1181,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="23">
@@ -1559,7 +1559,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1584,17 +1586,17 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="25" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1610,211 +1612,211 @@
         <v>31</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="26"/>
+      <c r="B3" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="25">
+        <v>3</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="26"/>
+      <c r="B6" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="25">
+        <v>2</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
-      <c r="B3" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="17">
-        <v>3</v>
-      </c>
-      <c r="D3" s="17" t="s">
+      <c r="G6" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+    </row>
+    <row r="8" spans="1:7" ht="144.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="26"/>
+      <c r="B9" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="25">
+        <v>2</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="1:7" ht="144" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="26"/>
+      <c r="B12" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="25">
+        <v>2</v>
+      </c>
+      <c r="D12" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-    </row>
-    <row r="5" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="17">
-        <v>2</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="26" t="s">
+      <c r="E12" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-    </row>
-    <row r="8" spans="1:7" ht="144.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
-      <c r="B9" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="17">
-        <v>2</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-    </row>
-    <row r="11" spans="1:7" ht="144" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="17">
-        <v>2</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="F12" s="31" t="s">
+      <c r="G12" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+    </row>
+    <row r="14" spans="1:7" ht="148.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="25">
+        <v>7</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-    </row>
-    <row r="14" spans="1:7" ht="148.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="17">
-        <v>7</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="26" t="s">
-        <v>74</v>
+      <c r="F15" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
     </row>
     <row r="17" spans="1:7" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="6" t="s">
         <v>30</v>
       </c>
@@ -1835,7 +1837,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="175.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="14" t="s">
         <v>29</v>
       </c>
@@ -1846,17 +1848,17 @@
         <v>1</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="158.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="10" t="s">
         <v>27</v>
       </c>
@@ -1867,527 +1869,527 @@
         <v>1</v>
       </c>
       <c r="E20" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="26"/>
+      <c r="B21" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="25">
+        <v>8</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="141" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="25">
+        <v>4</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+    </row>
+    <row r="25" spans="1:7" ht="145.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="26"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="26"/>
+      <c r="B26" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="25">
+        <v>6</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="154.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="26"/>
+      <c r="B28" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="25">
+        <v>5</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="149.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="26"/>
+      <c r="B30" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="25">
+        <v>5</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="145.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="26"/>
+      <c r="B32" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="25">
+        <v>5</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="129" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="25">
+        <v>4</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+    </row>
+    <row r="36" spans="1:7" ht="145.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="26"/>
+      <c r="B37" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="25">
+        <v>6</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F37" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="17" t="s">
+      <c r="G37" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="154.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="26"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="26"/>
+      <c r="B39" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="25">
+        <v>5</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="149.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="26"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="26"/>
+      <c r="B41" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="25">
+        <v>5</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="145.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="26"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="26"/>
+      <c r="B43" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="17">
-        <v>8</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="141" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="17">
-        <v>4</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-    </row>
-    <row r="25" spans="1:7" ht="145.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
-      <c r="B26" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="17">
-        <v>6</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="26" t="s">
+      <c r="C43" s="25">
+        <v>5</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F43" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="G26" s="26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="154.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
-      <c r="B28" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="17">
-        <v>5</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="F28" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="G28" s="26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="149.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="18"/>
-      <c r="B30" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="17">
-        <v>5</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="F30" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="G30" s="26" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="145.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="18"/>
-      <c r="B32" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="17">
-        <v>5</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="F32" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="G32" s="28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="129" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="17">
-        <v>4</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="F34" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="G34" s="26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-    </row>
-    <row r="36" spans="1:7" ht="145.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="18"/>
-      <c r="B37" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="17">
-        <v>6</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="F37" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="G37" s="26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="154.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="18"/>
-      <c r="B39" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39" s="17">
-        <v>5</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="F39" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="G39" s="26" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="149.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="18"/>
-      <c r="B41" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="17">
-        <v>5</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="F41" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="G41" s="26" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="145.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="18"/>
-      <c r="B43" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" s="17">
-        <v>5</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="F43" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="G43" s="28" t="s">
-        <v>105</v>
+      <c r="G43" s="19" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="129" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="23" t="s">
+      <c r="B45" s="31" t="s">
         <v>25</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
-      <c r="E45" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="F45" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="G45" s="31" t="s">
-        <v>93</v>
+      <c r="E45" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G45" s="21" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="21"/>
-      <c r="B46" s="24"/>
+      <c r="A46" s="29"/>
+      <c r="B46" s="32"/>
       <c r="C46" s="9">
         <v>4</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
     </row>
     <row r="47" spans="1:7" ht="139.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="21"/>
-      <c r="B47" s="25"/>
+      <c r="A47" s="29"/>
+      <c r="B47" s="33"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="21"/>
-      <c r="B48" s="23" t="s">
+      <c r="A48" s="29"/>
+      <c r="B48" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="17">
+      <c r="C48" s="25">
         <v>6</v>
       </c>
-      <c r="D48" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="F48" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="G48" s="26" t="s">
-        <v>91</v>
+      <c r="D48" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="G48" s="17" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="21"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="27"/>
+      <c r="A49" s="29"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="21"/>
-      <c r="B50" s="23" t="s">
+      <c r="A50" s="29"/>
+      <c r="B50" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="17">
-        <v>5</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="F50" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="G50" s="26" t="s">
-        <v>94</v>
+      <c r="C50" s="25">
+        <v>5</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="135.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="21"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="27"/>
+      <c r="A51" s="29"/>
+      <c r="B51" s="33"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="21"/>
-      <c r="B52" s="23" t="s">
+      <c r="A52" s="29"/>
+      <c r="B52" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C52" s="17">
-        <v>5</v>
-      </c>
-      <c r="D52" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E52" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="F52" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="G52" s="26" t="s">
-        <v>95</v>
+      <c r="C52" s="25">
+        <v>5</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G52" s="17" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="159.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="21"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="27"/>
+      <c r="A53" s="29"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="21"/>
-      <c r="B54" s="23" t="s">
+      <c r="A54" s="29"/>
+      <c r="B54" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C54" s="17">
-        <v>5</v>
-      </c>
-      <c r="D54" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E54" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="F54" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G54" s="26" t="s">
-        <v>92</v>
+      <c r="C54" s="25">
+        <v>5</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="149.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="22"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="27"/>
+      <c r="A55" s="30"/>
+      <c r="B55" s="33"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
     </row>
     <row r="58" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
@@ -2416,6 +2418,111 @@
     </row>
   </sheetData>
   <mergeCells count="129">
+    <mergeCell ref="A23:A33"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A15:A22"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="A45:A55"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="A34:A44"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="F30:F31"/>
     <mergeCell ref="G54:G55"/>
     <mergeCell ref="G43:G44"/>
     <mergeCell ref="G45:G47"/>
@@ -2440,111 +2547,6 @@
     <mergeCell ref="G41:G42"/>
     <mergeCell ref="F43:F44"/>
     <mergeCell ref="F45:F47"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="A34:A44"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="E45:E47"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="A45:A55"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="A15:A22"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="A2:A14"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="A23:A33"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>